<commit_message>
update Bundes output files
</commit_message>
<xml_diff>
--- a/FantaSoccer/MyModule/Bundesliga/xGA_away_all_14.xlsx
+++ b/FantaSoccer/MyModule/Bundesliga/xGA_away_all_14.xlsx
@@ -537,16 +537,16 @@
         <v>2.815351</v>
       </c>
       <c r="G2">
-        <v>5.592830999999999</v>
+        <v>5.592831</v>
       </c>
       <c r="H2">
-        <v>5.592830999999999</v>
+        <v>5.592831</v>
       </c>
       <c r="I2">
-        <v>7.844491</v>
+        <v>7.844491000000001</v>
       </c>
       <c r="J2">
-        <v>7.844491</v>
+        <v>7.844491000000001</v>
       </c>
       <c r="K2">
         <v>10.686201</v>
@@ -819,16 +819,16 @@
         <v>2.97689</v>
       </c>
       <c r="G8">
-        <v>6.785120000000001</v>
+        <v>6.78512</v>
       </c>
       <c r="H8">
-        <v>6.785120000000001</v>
+        <v>6.78512</v>
       </c>
       <c r="I8">
-        <v>8.870920000000002</v>
+        <v>8.87092</v>
       </c>
       <c r="J8">
-        <v>8.870920000000002</v>
+        <v>8.87092</v>
       </c>
       <c r="K8">
         <v>10.82948</v>
@@ -878,19 +878,19 @@
         <v>2.236601</v>
       </c>
       <c r="K9">
-        <v>4.997011</v>
+        <v>4.997011000000001</v>
       </c>
       <c r="L9">
-        <v>4.997011</v>
+        <v>4.997011000000001</v>
       </c>
       <c r="M9">
-        <v>6.258700999999999</v>
+        <v>6.258701</v>
       </c>
       <c r="N9">
-        <v>6.258700999999999</v>
+        <v>6.258701</v>
       </c>
       <c r="O9">
-        <v>7.837090999999999</v>
+        <v>7.837091</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -954,28 +954,28 @@
         <v>0.495892</v>
       </c>
       <c r="E11">
-        <v>4.489001999999999</v>
+        <v>4.489002</v>
       </c>
       <c r="F11">
-        <v>4.489001999999999</v>
+        <v>4.489002</v>
       </c>
       <c r="G11">
-        <v>7.174231999999999</v>
+        <v>7.174232</v>
       </c>
       <c r="H11">
-        <v>7.174231999999999</v>
+        <v>7.174232</v>
       </c>
       <c r="I11">
-        <v>7.524832999999999</v>
+        <v>7.524833</v>
       </c>
       <c r="J11">
-        <v>7.524832999999999</v>
+        <v>7.524833</v>
       </c>
       <c r="K11">
-        <v>8.566792999999999</v>
+        <v>8.566793000000001</v>
       </c>
       <c r="L11">
-        <v>8.566792999999999</v>
+        <v>8.566793000000001</v>
       </c>
       <c r="M11">
         <v>9.926613</v>
@@ -1142,16 +1142,16 @@
         <v>4.620880000000001</v>
       </c>
       <c r="E15">
-        <v>7.87924</v>
+        <v>7.879240000000001</v>
       </c>
       <c r="F15">
-        <v>7.87924</v>
+        <v>7.879240000000001</v>
       </c>
       <c r="G15">
-        <v>9.36308</v>
+        <v>9.363080000000002</v>
       </c>
       <c r="H15">
-        <v>9.36308</v>
+        <v>9.363080000000002</v>
       </c>
       <c r="I15">
         <v>12.72679</v>
@@ -1266,7 +1266,7 @@
         <v>6.378288</v>
       </c>
       <c r="O17">
-        <v>8.053547999999999</v>
+        <v>8.053548000000001</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1301,10 +1301,10 @@
         <v>6.90086</v>
       </c>
       <c r="K18">
-        <v>8.437720000000001</v>
+        <v>8.437719999999999</v>
       </c>
       <c r="L18">
-        <v>8.437720000000001</v>
+        <v>8.437719999999999</v>
       </c>
       <c r="M18">
         <v>10.83879</v>

</xml_diff>